<commit_message>
batch update of stuff
</commit_message>
<xml_diff>
--- a/data-raw/ps_data_version/ps_data_version.xlsx
+++ b/data-raw/ps_data_version/ps_data_version.xlsx
@@ -365,7 +365,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -579,7 +579,7 @@
         <v>41</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>42</v>

</xml_diff>

<commit_message>
add cow alliance citation
</commit_message>
<xml_diff>
--- a/data-raw/ps_data_version/ps_data_version.xlsx
+++ b/data-raw/ps_data_version/ps_data_version.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="84">
   <si>
     <t xml:space="preserve">category</t>
   </si>
@@ -65,6 +65,12 @@
   </si>
   <si>
     <t xml:space="preserve">leedsetal2002atop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correlates of War Formal Alliances</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gibler2009ima</t>
   </si>
   <si>
     <t xml:space="preserve">democracy</t>
@@ -362,10 +368,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topLeft" activeCell="M8" activeCellId="0" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -447,41 +453,41 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="C6" s="0" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>2017</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>21</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <v>10</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>22</v>
@@ -489,58 +495,58 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="C9" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="C9" s="0" t="n">
-        <v>2020</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="C10" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="D10" s="0" t="s">
         <v>27</v>
-      </c>
-      <c r="C10" s="0" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="C11" s="0" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="D11" s="0" t="s">
         <v>30</v>
-      </c>
-      <c r="C11" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="C12" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D12" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="C12" s="0" t="n">
-        <v>2016</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -551,119 +557,119 @@
         <v>35</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>5</v>
+        <v>2016</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="C14" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D14" s="0" t="s">
         <v>38</v>
-      </c>
-      <c r="C14" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="C15" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D15" s="0" t="s">
         <v>41</v>
-      </c>
-      <c r="C15" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="C16" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D16" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="C16" s="0" t="n">
-        <v>2020</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="0" t="s">
         <v>46</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>44</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>2020</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>2020</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>4</v>
+        <v>2020</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="C20" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D20" s="0" t="s">
         <v>52</v>
-      </c>
-      <c r="C20" s="0" t="n">
-        <v>4.1</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>54</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>4</v>
+        <v>4.1</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>55</v>
@@ -671,55 +677,55 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="C22" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D22" s="0" t="s">
         <v>57</v>
-      </c>
-      <c r="C22" s="0" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="0" t="s">
         <v>59</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>57</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>2012</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="B24" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D24" s="0" t="s">
         <v>60</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="B25" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="0" t="s">
         <v>63</v>
-      </c>
-      <c r="C25" s="0" t="n">
-        <v>2017</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>64</v>
@@ -727,13 +733,13 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>65</v>
       </c>
       <c r="C26" s="0" t="n">
-        <v>2020</v>
+        <v>2017</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>66</v>
@@ -741,27 +747,27 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="C27" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="D27" s="0" t="s">
         <v>68</v>
-      </c>
-      <c r="C27" s="0" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>70</v>
       </c>
       <c r="C28" s="0" t="n">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="D28" s="0" t="s">
         <v>71</v>
@@ -769,27 +775,27 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="C29" s="0" t="n">
+        <v>2014</v>
+      </c>
+      <c r="D29" s="0" t="s">
         <v>73</v>
-      </c>
-      <c r="C29" s="0" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>75</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>20.1</v>
+        <v>2012</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>76</v>
@@ -797,13 +803,13 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>77</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>19.1</v>
+        <v>20.1</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>78</v>
@@ -811,16 +817,30 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="C32" s="0" t="n">
+        <v>19.1</v>
+      </c>
+      <c r="D32" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="C32" s="0" t="n">
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C33" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="D32" s="0" t="s">
-        <v>81</v>
+      <c r="D33" s="0" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>